<commit_message>
remove incorrect risk adjustment
</commit_message>
<xml_diff>
--- a/SPRB.xlsx
+++ b/SPRB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdl/Documents/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4678D86C-F8DE-824A-BFF0-59BB72209C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF667D9-4E7B-A744-833A-0F3B669E4360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="620" windowWidth="50600" windowHeight="26360" activeTab="1" xr2:uid="{D7E1BACE-2359-D64B-91EE-3C4F53AFF46B}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="50600" windowHeight="26360" xr2:uid="{D7E1BACE-2359-D64B-91EE-3C4F53AFF46B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>COGS</t>
   </si>
@@ -182,13 +182,7 @@
     <t>Model doesn't account Tildacerfont/ Cortibon trial</t>
   </si>
   <si>
-    <t>Probability of Success</t>
-  </si>
-  <si>
     <t>At the end of the IP exclusivity period, model for erosion (-35%, -20%, -20%, -10%+)</t>
-  </si>
-  <si>
-    <t>Risk-Adj. NI</t>
   </si>
 </sst>
 </file>
@@ -317,7 +311,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -344,6 +338,10 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -756,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000C3FC5-45B7-804F-BAC7-6E46AF3AFBD9}">
   <dimension ref="B3:I47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,6 +961,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="25">
+        <f>1298325</f>
         <v>1298325</v>
       </c>
     </row>
@@ -1004,13 +1003,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F22E3D-7CD6-684C-96B5-393F273B0779}">
-  <dimension ref="B2:AS28"/>
+  <dimension ref="B2:AS27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1944,13 +1943,34 @@
         <f t="shared" si="10"/>
         <v>85.020589999999984</v>
       </c>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
+      <c r="P18" s="1">
+        <f>O18*0.65</f>
+        <v>55.263383499999989</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>P18*0.8</f>
+        <v>44.210706799999997</v>
+      </c>
+      <c r="R18" s="1">
+        <f>Q18*0.8</f>
+        <v>35.368565439999998</v>
+      </c>
+      <c r="S18" s="1">
+        <f>R18*0.9</f>
+        <v>31.831708895999999</v>
+      </c>
+      <c r="T18" s="1">
+        <f>S18*0.9</f>
+        <v>28.648538006399999</v>
+      </c>
+      <c r="U18" s="1">
+        <f>T18*0.9</f>
+        <v>25.78368420576</v>
+      </c>
+      <c r="V18" s="1">
+        <f>U18*0.9</f>
+        <v>23.205315785184002</v>
+      </c>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
@@ -1975,186 +1995,62 @@
       <c r="AR18" s="12"/>
       <c r="AS18" s="12"/>
     </row>
-    <row r="19" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="20" spans="2:45" x14ac:dyDescent="0.2">
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="P20" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3">
-        <v>1</v>
-      </c>
-      <c r="N19" s="3">
-        <v>1</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1</v>
-      </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-    </row>
-    <row r="20" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="1">
-        <f>D18*D19</f>
-        <v>-44.499650000000003</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" ref="E20:O20" si="11">E18*E19</f>
-        <v>-19.201750000000004</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="11"/>
-        <v>18.29487499999999</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="11"/>
-        <v>40.674499999999995</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="11"/>
-        <v>34.01275875000001</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="11"/>
-        <v>62.882716250000001</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="11"/>
-        <v>59.899380000000022</v>
-      </c>
-      <c r="K20" s="1">
-        <f t="shared" si="11"/>
-        <v>80.56262000000001</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="11"/>
-        <v>64.762620000000013</v>
-      </c>
-      <c r="M20" s="1">
-        <f t="shared" si="11"/>
-        <v>69.220589999999987</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="11"/>
-        <v>69.220589999999987</v>
-      </c>
-      <c r="O20" s="1">
-        <f t="shared" si="11"/>
-        <v>85.020589999999984</v>
-      </c>
-      <c r="P20" s="1">
-        <f>O20*0.65</f>
-        <v>55.263383499999989</v>
-      </c>
-      <c r="Q20" s="1">
-        <f>P20*0.8</f>
-        <v>44.210706799999997</v>
-      </c>
-      <c r="R20" s="1">
-        <f>Q20*0.8</f>
-        <v>35.368565439999998</v>
-      </c>
-      <c r="S20" s="1">
-        <f>R20*0.9</f>
-        <v>31.831708895999999</v>
-      </c>
-      <c r="T20" s="1">
-        <f>S20*0.9</f>
-        <v>28.648538006399999</v>
-      </c>
-      <c r="U20" s="1">
-        <f>T20*0.9</f>
-        <v>25.78368420576</v>
-      </c>
-      <c r="V20" s="1">
-        <f>U20*0.9</f>
-        <v>23.205315785184002</v>
+    </row>
+    <row r="21" spans="2:45" x14ac:dyDescent="0.2">
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="18">
+        <v>66.3</v>
       </c>
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.2">
       <c r="C22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="17">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="P22" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="D22" s="21">
+        <f>Main!$C$18/1000000</f>
+        <v>1.298325</v>
       </c>
     </row>
     <row r="23" spans="2:45" x14ac:dyDescent="0.2">
       <c r="C23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="18">
-        <v>66.3</v>
+        <v>14</v>
+      </c>
+      <c r="D23" s="8">
+        <f xml:space="preserve"> NPV($D$20,D18:V18)+$D$21</f>
+        <v>330.66099766539497</v>
       </c>
     </row>
     <row r="24" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="21">
-        <f>Main!$C$18/1000000</f>
-        <v>1.298325</v>
+      <c r="C24" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="19">
+        <f>D23/D22</f>
+        <v>254.68276253279802</v>
       </c>
     </row>
     <row r="25" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="8">
-        <f>NPV($D$22, D20:AS20)+$D$23</f>
-        <v>352.54350908092005</v>
-      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C26" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="19">
-        <f>D25/D24</f>
-        <v>271.53717989018162</v>
-      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
     </row>
     <row r="27" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C28" s="4"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add note on model
</commit_message>
<xml_diff>
--- a/SPRB.xlsx
+++ b/SPRB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdl/Documents/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF667D9-4E7B-A744-833A-0F3B669E4360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA6D38-EEF1-204B-BEE1-C5948BEBDFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="50600" windowHeight="26360" xr2:uid="{D7E1BACE-2359-D64B-91EE-3C4F53AFF46B}"/>
+    <workbookView xWindow="600" yWindow="620" windowWidth="50000" windowHeight="26360" xr2:uid="{D7E1BACE-2359-D64B-91EE-3C4F53AFF46B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>COGS</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>At the end of the IP exclusivity period, model for erosion (-35%, -20%, -20%, -10%+)</t>
+  </si>
+  <si>
+    <t>&lt;- model for more dilution</t>
+  </si>
+  <si>
+    <t>Note: need to re-model the patient pool. Currently only taking infants born w/ sanfillipo, not accounting for current prevalence &amp; death rate</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,7 +323,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -338,10 +350,10 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -755,7 +767,7 @@
   <dimension ref="B3:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,13 +973,21 @@
         <v>17</v>
       </c>
       <c r="C18" s="25">
-        <f>1298325</f>
-        <v>1298325</v>
+        <f>1298325*2</f>
+        <v>2596650</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="B21" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -2020,7 +2040,7 @@
       </c>
       <c r="D22" s="21">
         <f>Main!$C$18/1000000</f>
-        <v>1.298325</v>
+        <v>2.5966499999999999</v>
       </c>
     </row>
     <row r="23" spans="2:45" x14ac:dyDescent="0.2">
@@ -2038,19 +2058,18 @@
       </c>
       <c r="D24" s="19">
         <f>D23/D22</f>
-        <v>254.68276253279802</v>
+        <v>127.34138126639901</v>
       </c>
     </row>
     <row r="25" spans="2:45" x14ac:dyDescent="0.2">
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C26" s="26"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="2:45" x14ac:dyDescent="0.2">
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>